<commit_message>
Sigo añadiendo cositas que nos vendran bien
Los valores de coste de los personajes esta bien tenerlos tambien en la
info de estos
</commit_message>
<xml_diff>
--- a/Info Personajes.xlsx
+++ b/Info Personajes.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Vida</t>
   </si>
@@ -46,6 +46,18 @@
   </si>
   <si>
     <t>Soldado</t>
+  </si>
+  <si>
+    <t>Precio Oro</t>
+  </si>
+  <si>
+    <t>Precio Hierro</t>
+  </si>
+  <si>
+    <t>Precio Comida</t>
+  </si>
+  <si>
+    <t>Consumo Comida</t>
   </si>
 </sst>
 </file>
@@ -377,18 +389,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:10">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -404,8 +420,20 @@
       <c r="F1" t="s">
         <v>4</v>
       </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -425,7 +453,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -445,7 +473,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -465,7 +493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -473,7 +501,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
Actualizacion de info personajes
Lo que hicimos en serranillos
</commit_message>
<xml_diff>
--- a/Info Personajes.xlsx
+++ b/Info Personajes.xlsx
@@ -16,14 +16,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="59">
   <si>
     <t>Vida</t>
   </si>
   <si>
-    <t>Ataque</t>
-  </si>
-  <si>
     <t>Rango</t>
   </si>
   <si>
@@ -58,13 +55,151 @@
   </si>
   <si>
     <t>Consumo Comida</t>
+  </si>
+  <si>
+    <t>EDIFICIOS</t>
+  </si>
+  <si>
+    <t>150 + 20%</t>
+  </si>
+  <si>
+    <t>200+15%</t>
+  </si>
+  <si>
+    <t>3+2%</t>
+  </si>
+  <si>
+    <t>200+20%</t>
+  </si>
+  <si>
+    <t>Valor</t>
+  </si>
+  <si>
+    <t>300+25%</t>
+  </si>
+  <si>
+    <t>200+17,5%</t>
+  </si>
+  <si>
+    <t>3+5%</t>
+  </si>
+  <si>
+    <t>10+10%</t>
+  </si>
+  <si>
+    <t>250+15%</t>
+  </si>
+  <si>
+    <t>200+12,5%</t>
+  </si>
+  <si>
+    <t>100+15%</t>
+  </si>
+  <si>
+    <t>1000+30%</t>
+  </si>
+  <si>
+    <t>100+20%</t>
+  </si>
+  <si>
+    <t>PERSONAJES (Niveles 1-4)</t>
+  </si>
+  <si>
+    <t>3+30%</t>
+  </si>
+  <si>
+    <t>4,5+15%</t>
+  </si>
+  <si>
+    <t>Salpicadura</t>
+  </si>
+  <si>
+    <t>0+1</t>
+  </si>
+  <si>
+    <t>Granja</t>
+  </si>
+  <si>
+    <t>Mina Oro</t>
+  </si>
+  <si>
+    <t>Mina Hierro</t>
+  </si>
+  <si>
+    <t>Cuartel</t>
+  </si>
+  <si>
+    <t>Ayuntamiento</t>
+  </si>
+  <si>
+    <t>Generacion / min</t>
+  </si>
+  <si>
+    <t>Tiempo Constr</t>
+  </si>
+  <si>
+    <t>Aserradero</t>
+  </si>
+  <si>
+    <t>Precio Madera</t>
+  </si>
+  <si>
+    <t>80+30</t>
+  </si>
+  <si>
+    <t>60+20</t>
+  </si>
+  <si>
+    <t>40+20</t>
+  </si>
+  <si>
+    <t>Numero max</t>
+  </si>
+  <si>
+    <t>2+1</t>
+  </si>
+  <si>
+    <t>1+1</t>
+  </si>
+  <si>
+    <t>Precio Nivel (oro)</t>
+  </si>
+  <si>
+    <t>40+80%</t>
+  </si>
+  <si>
+    <t>40+50%</t>
+  </si>
+  <si>
+    <t>50+80%</t>
+  </si>
+  <si>
+    <t>100+50%</t>
+  </si>
+  <si>
+    <t>50+50%</t>
+  </si>
+  <si>
+    <t>150+50%</t>
+  </si>
+  <si>
+    <t>100+100%</t>
+  </si>
+  <si>
+    <t>200+100%</t>
+  </si>
+  <si>
+    <t>150+100%</t>
+  </si>
+  <si>
+    <t>Ataque/ segundo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -72,13 +207,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -93,8 +247,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -389,125 +556,446 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A2:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="B1" t="s">
+    <row r="2" spans="1:13">
+      <c r="A2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="B4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="2">
+        <v>5</v>
+      </c>
+      <c r="H5" s="2">
+        <v>6</v>
+      </c>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="K5" t="s">
+        <v>50</v>
+      </c>
+      <c r="L5" s="5"/>
+      <c r="M5" s="6"/>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="2">
+        <v>8</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="2">
+        <v>2</v>
+      </c>
+      <c r="H6" s="2">
+        <v>6</v>
+      </c>
+      <c r="I6" s="2">
+        <v>1</v>
+      </c>
+      <c r="J6" s="2">
+        <v>4</v>
+      </c>
+      <c r="K6" t="s">
+        <v>50</v>
+      </c>
+      <c r="L6" s="5"/>
+      <c r="M6" s="6"/>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="2">
+        <v>2</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="2">
+        <v>6</v>
+      </c>
+      <c r="H7" s="2">
+        <v>8</v>
+      </c>
+      <c r="I7" s="2">
+        <v>4</v>
+      </c>
+      <c r="J7" s="2">
+        <v>8</v>
+      </c>
+      <c r="K7" t="s">
+        <v>53</v>
+      </c>
+      <c r="L7" s="5"/>
+      <c r="M7" s="6"/>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="2">
+        <v>7</v>
+      </c>
+      <c r="H8" s="2">
+        <v>7</v>
+      </c>
+      <c r="I8" s="2">
+        <v>4</v>
+      </c>
+      <c r="J8" s="2">
+        <v>8</v>
+      </c>
+      <c r="K8" t="s">
+        <v>52</v>
+      </c>
+      <c r="L8" s="5"/>
+      <c r="M8" s="6"/>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="2">
+        <v>3</v>
+      </c>
+      <c r="E9" s="2">
+        <v>3</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H9" s="2">
         <v>10</v>
       </c>
-      <c r="H1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="I9" s="2">
+        <v>2</v>
+      </c>
+      <c r="J9" s="2">
+        <v>10</v>
+      </c>
+      <c r="K9" t="s">
+        <v>54</v>
+      </c>
+      <c r="L9" s="5"/>
+      <c r="M9" s="6"/>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2">
-        <v>150</v>
-      </c>
-      <c r="C2">
-        <v>200</v>
-      </c>
-      <c r="D2">
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="B15" t="s">
         <v>10</v>
       </c>
-      <c r="E2">
-        <v>3</v>
-      </c>
-      <c r="F2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3">
-        <v>200</v>
-      </c>
-      <c r="C3">
-        <v>200</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3">
-        <v>10</v>
-      </c>
-      <c r="F3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4">
-        <v>1000</v>
-      </c>
-      <c r="C4">
-        <v>100</v>
-      </c>
-      <c r="D4">
-        <v>3</v>
-      </c>
-      <c r="E4">
+      <c r="C15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G15" t="s">
+        <v>0</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16" s="6"/>
+      <c r="E16" t="s">
+        <v>42</v>
+      </c>
+      <c r="F16" s="6"/>
+      <c r="H16" t="s">
+        <v>46</v>
+      </c>
+      <c r="I16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" s="6"/>
+      <c r="E17" t="s">
+        <v>44</v>
+      </c>
+      <c r="F17" s="6"/>
+      <c r="H17" t="s">
+        <v>46</v>
+      </c>
+      <c r="I17" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18" s="6"/>
+      <c r="E18" t="s">
+        <v>43</v>
+      </c>
+      <c r="F18" s="6"/>
+      <c r="H18" t="s">
+        <v>46</v>
+      </c>
+      <c r="I18" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" t="s">
+        <v>57</v>
+      </c>
+      <c r="D19" s="6"/>
+      <c r="E19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F19" s="6"/>
+      <c r="H19" t="s">
+        <v>47</v>
+      </c>
+      <c r="I19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="H21">
         <v>1</v>
       </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:J3"/>
+    <mergeCell ref="A12:J13"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>